<commit_message>
Updated the .xlsx floor files.
</commit_message>
<xml_diff>
--- a/floorEasy.xlsx
+++ b/floorEasy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSpie\Documents\_College\CSCI 306\Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Fall '15\Software Engineering\Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="5">
   <si>
     <t>W</t>
   </si>
@@ -37,12 +37,15 @@
   <si>
     <t>A</t>
   </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,7 +55,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -60,25 +63,26 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF318B9A"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -98,8 +102,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -107,37 +123,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -427,16 +435,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection sqref="A1:Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="26" width="4.28515625" customWidth="1"/>
+    <col min="1" max="26" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -512,45 +520,45 @@
       <c r="Y1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z1">
+      <c r="Z1" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -559,32 +567,32 @@
       <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>1</v>
+      <c r="O2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>3</v>
@@ -592,42 +600,42 @@
       <c r="Y2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -639,7 +647,7 @@
       <c r="N3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -666,21 +674,21 @@
       <c r="W3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>1</v>
+      <c r="X3" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -704,345 +712,345 @@
       <c r="I4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="J4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2" t="s">
+      <c r="O4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="X4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2" t="s">
+      <c r="O5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X5" s="2" t="s">
+      <c r="X5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="F6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2" t="s">
+      <c r="O6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X6" s="2" t="s">
+      <c r="X6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="F7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="J7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2" t="s">
+      <c r="O7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X7" s="2" t="s">
+      <c r="X7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="2" t="s">
+      <c r="O8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="s">
@@ -1066,152 +1074,152 @@
       <c r="W8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="X8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="J9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>0</v>
+      <c r="M9" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P9" s="2" t="s">
+      <c r="O9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2" t="s">
+      <c r="R9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="J10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="M10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2" t="s">
+      <c r="O10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S10" s="2" t="s">
+      <c r="R10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T10" s="1" t="s">
@@ -1226,152 +1234,152 @@
       <c r="W10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="J11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2" t="s">
+      <c r="O11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2" t="s">
+      <c r="R11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X11" s="2" t="s">
+      <c r="U11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="J12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="2" t="s">
+      <c r="O12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S12" s="2" t="s">
+      <c r="R12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T12" s="1" t="s">
@@ -1392,21 +1400,21 @@
       <c r="Y12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1418,40 +1426,40 @@
       <c r="G13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="J13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2" t="s">
+      <c r="O13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T13" s="1" t="s">
@@ -1460,33 +1468,33 @@
       <c r="U13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="V13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X13" s="2" t="s">
+      <c r="V13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1498,16 +1506,16 @@
       <c r="G14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2" t="s">
+      <c r="J14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1519,19 +1527,19 @@
       <c r="N14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="s">
+      <c r="O14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S14" s="2" t="s">
+      <c r="R14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="T14" s="1" t="s">
@@ -1543,20 +1551,20 @@
       <c r="V14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X14" s="2" t="s">
+      <c r="W14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1566,7 +1574,7 @@
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1578,81 +1586,81 @@
       <c r="G15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="2" t="s">
+      <c r="H15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U15" s="4" t="s">
+      <c r="R15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X15" s="2" t="s">
+      <c r="W15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1703,208 +1711,208 @@
       <c r="V16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X16" s="2" t="s">
+      <c r="W16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="F17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R17" s="2" t="s">
+      <c r="J17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U17" s="2" t="s">
+      <c r="T17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X17" s="2" t="s">
+      <c r="W17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2" t="s">
+      <c r="J18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R18" s="2" t="s">
+      <c r="Q18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U18" s="2" t="s">
+      <c r="T18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X18" s="2" t="s">
+      <c r="W18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
@@ -1916,51 +1924,51 @@
       <c r="M19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" s="2" t="s">
+      <c r="N19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R19" s="2" t="s">
+      <c r="Q19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U19" s="2" t="s">
+      <c r="T19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X19" s="2" t="s">
+      <c r="W19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1972,78 +1980,78 @@
       <c r="E20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>0</v>
+      <c r="J20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O20" s="2" t="s">
+      <c r="N20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R20" s="2" t="s">
+      <c r="Q20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U20" s="2" t="s">
+      <c r="T20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X20" s="2" t="s">
+      <c r="W20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -2052,93 +2060,93 @@
       <c r="E21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="4" t="s">
+      <c r="J21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>2</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O21" s="2" t="s">
+      <c r="N21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R21" s="2" t="s">
+      <c r="Q21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U21" s="2" t="s">
+      <c r="T21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X21" s="2" t="s">
+      <c r="W21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -2156,207 +2164,207 @@
       <c r="M22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2" t="s">
+      <c r="N22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R22" s="2" t="s">
+      <c r="Q22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U22" s="2" t="s">
+      <c r="T22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="V22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="W22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X22" s="2" t="s">
+      <c r="W22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="B23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" s="2" t="s">
+      <c r="H23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X23" s="2" t="s">
+      <c r="Q23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O24" s="2" t="s">
+      <c r="H24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="V24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="W24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="X24" s="2" t="s">
-        <v>0</v>
+      <c r="Q24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="T24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="U24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2432,86 +2440,87 @@
       <c r="Y25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
+    <row r="26" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
         <v>2</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>3</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>5</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>6</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <v>7</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <v>8</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <v>9</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
         <v>10</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="2">
         <v>11</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="2">
         <v>12</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="2">
         <v>13</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="2">
         <v>14</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="2">
         <v>15</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="2">
         <v>16</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="2">
         <v>17</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="2">
         <v>18</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="2">
         <v>19</v>
       </c>
-      <c r="U26">
+      <c r="U26" s="2">
         <v>20</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="2">
         <v>21</v>
       </c>
-      <c r="W26">
+      <c r="W26" s="2">
         <v>22</v>
       </c>
-      <c r="X26">
+      <c r="X26" s="2">
         <v>23</v>
       </c>
-      <c r="Y26">
+      <c r="Y26" s="2">
         <v>24</v>
       </c>
+      <c r="Z26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>